<commit_message>
with distnce, but not right
</commit_message>
<xml_diff>
--- a/SampleDataWithAircraftType.xlsx
+++ b/SampleDataWithAircraftType.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyDocs\AcademicsTUDelft\Semester 1\AE4441-16\Project\CPlex\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lunap\OneDrive\Ambiente de Trabalho\1st quarter\Operations optimisation\Operations_assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1EFD35C4-E126-4F3F-B8D0-BF921D077A40}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="8_{1EFD35C4-E126-4F3F-B8D0-BF921D077A40}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{D0C662F7-1D7E-4E50-A9FE-86DCAA309816}"/>
   <bookViews>
-    <workbookView xWindow="2328" yWindow="1908" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>Flight number</t>
   </si>
@@ -73,6 +73,21 @@
   </si>
   <si>
     <t>B737</t>
+  </si>
+  <si>
+    <t>Terminal</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
   </si>
 </sst>
 </file>
@@ -394,10 +409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -408,7 +423,7 @@
     <col min="4" max="4" width="11.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -424,8 +439,11 @@
       <c r="E1" t="s">
         <v>7</v>
       </c>
+      <c r="F1" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -443,8 +461,11 @@
       <c r="E2" t="s">
         <v>8</v>
       </c>
+      <c r="F2" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -462,8 +483,11 @@
       <c r="E3" t="s">
         <v>9</v>
       </c>
+      <c r="F3" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -481,8 +505,11 @@
       <c r="E4" t="s">
         <v>10</v>
       </c>
+      <c r="F4" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -500,8 +527,11 @@
       <c r="E5" t="s">
         <v>13</v>
       </c>
+      <c r="F5" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -518,6 +548,9 @@
       </c>
       <c r="E6" t="s">
         <v>8</v>
+      </c>
+      <c r="F6" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>